<commit_message>
Moved To Comp Bot
This contains the prototype arm code. Please be aware that this prototype code is basic, please add in the functionality that is needed.

Also please be aware that the Mapings has been updated for the CAN Talons, this is where I have set them.
</commit_message>
<xml_diff>
--- a/Check Sheets/Mappings.xlsx
+++ b/Check Sheets/Mappings.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54951D64-8E1C-4756-806D-EC4FA1B2C6BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774944FB-472D-4340-BA08-2E7FF9DBBF9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CANTalonSRX" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Function</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>PCM</t>
+  </si>
+  <si>
+    <t>ArmLift</t>
+  </si>
+  <si>
+    <t>RobotLift1</t>
+  </si>
+  <si>
+    <t>BallIntake</t>
+  </si>
+  <si>
+    <t>RobotLift2</t>
+  </si>
+  <si>
+    <t>RobotLiftExtend</t>
   </si>
 </sst>
 </file>
@@ -395,16 +410,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.3984375" customWidth="1"/>
-    <col min="3" max="3" width="37.3984375" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -486,18 +501,43 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
       <c r="B10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
       <c r="B11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
       <c r="B12">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>